<commit_message>
updated pct spending on DoggyBFF as per group discussion
</commit_message>
<xml_diff>
--- a/data/assumptions.xlsx
+++ b/data/assumptions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkodwyer/Documents/UTS/36109_DADM/AT2/dadm_at2_rcode/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rkodwyer/Documents/UTS/36109_DADM/AT2/dadm_at2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A57004-7C62-4A45-A078-133764E2B18F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A78F69B-DDA0-4442-8DA4-6D94242035A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23260" yWindow="460" windowWidth="15080" windowHeight="19440" activeTab="1" xr2:uid="{C3939BD7-CB8E-2B45-BF96-55DB011C29C4}"/>
+    <workbookView xWindow="23260" yWindow="460" windowWidth="15080" windowHeight="16200" xr2:uid="{C3939BD7-CB8E-2B45-BF96-55DB011C29C4}"/>
   </bookViews>
   <sheets>
     <sheet name="revenue" sheetId="2" r:id="rId1"/>
@@ -196,7 +196,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -231,9 +231,8 @@
     <xf numFmtId="1" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,6 +263,7 @@
       <sheetName val="3b_dog_spend"/>
       <sheetName val="3c_service_providers"/>
       <sheetName val="4a_cloud_architecture"/>
+      <sheetName val="Competitors"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -281,24 +281,24 @@
         </row>
         <row r="7">
           <cell r="D7">
-            <v>1464.3</v>
+            <v>1493.3076923076926</v>
           </cell>
           <cell r="E7">
-            <v>1627</v>
+            <v>1659.2307692307695</v>
           </cell>
           <cell r="F7">
-            <v>1789.7</v>
+            <v>1825.1538461538466</v>
           </cell>
         </row>
         <row r="8">
           <cell r="D8">
-            <v>0.1</v>
+            <v>4.7009735744089003E-2</v>
           </cell>
           <cell r="E8">
-            <v>0.2</v>
+            <v>0.16054705609643019</v>
           </cell>
           <cell r="F8">
-            <v>0.5</v>
+            <v>0.29418173388966151</v>
           </cell>
         </row>
         <row r="9">
@@ -312,83 +312,83 @@
             <v>0.08</v>
           </cell>
         </row>
+        <row r="10">
+          <cell r="D10">
+            <v>0.02</v>
+          </cell>
+          <cell r="E10">
+            <v>0.04</v>
+          </cell>
+          <cell r="F10">
+            <v>0.06</v>
+          </cell>
+        </row>
         <row r="11">
           <cell r="D11">
-            <v>0.02</v>
+            <v>20</v>
           </cell>
           <cell r="E11">
-            <v>0.04</v>
+            <v>35</v>
           </cell>
           <cell r="F11">
-            <v>0.06</v>
+            <v>50</v>
           </cell>
         </row>
         <row r="12">
           <cell r="D12">
-            <v>20</v>
+            <v>0.05</v>
           </cell>
           <cell r="E12">
-            <v>35</v>
+            <v>0.15</v>
           </cell>
           <cell r="F12">
+            <v>0.25</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="D13">
             <v>50</v>
           </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>0.05</v>
-          </cell>
-          <cell r="E14">
-            <v>0.15</v>
-          </cell>
-          <cell r="F14">
-            <v>0.25</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>50</v>
-          </cell>
-          <cell r="E15">
+          <cell r="E13">
             <v>100</v>
           </cell>
-          <cell r="F15">
+          <cell r="F13">
             <v>200</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
       <sheetData sheetId="3">
-        <row r="15">
-          <cell r="D15">
-            <v>37500</v>
-          </cell>
-          <cell r="E15">
-            <v>55750</v>
-          </cell>
-          <cell r="F15">
-            <v>70250</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="D23">
+        <row r="16">
+          <cell r="D16">
+            <v>57500</v>
+          </cell>
+          <cell r="E16">
+            <v>80750</v>
+          </cell>
+          <cell r="F16">
+            <v>105250</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="D24">
             <v>6852</v>
           </cell>
-          <cell r="E23">
+          <cell r="E24">
             <v>9312</v>
           </cell>
-          <cell r="F23">
+          <cell r="F24">
             <v>17004</v>
           </cell>
         </row>
-        <row r="28">
-          <cell r="D28">
+        <row r="29">
+          <cell r="D29">
             <v>30</v>
           </cell>
-          <cell r="E28">
+          <cell r="E29">
             <v>35</v>
           </cell>
-          <cell r="F28">
+          <cell r="F29">
             <v>40</v>
           </cell>
         </row>
@@ -397,95 +397,95 @@
             <v>99</v>
           </cell>
         </row>
-        <row r="36">
-          <cell r="E36">
+        <row r="34">
+          <cell r="E34">
             <v>25</v>
           </cell>
         </row>
-        <row r="41">
-          <cell r="E41">
+        <row r="38">
+          <cell r="E38">
             <v>0.3</v>
           </cell>
         </row>
-        <row r="42">
-          <cell r="E42">
+        <row r="39">
+          <cell r="E39">
             <v>2.5999999999999999E-2</v>
           </cell>
         </row>
-        <row r="46">
-          <cell r="D46">
+        <row r="43">
+          <cell r="D43">
             <v>10</v>
           </cell>
-          <cell r="E46">
+          <cell r="E43">
             <v>25</v>
           </cell>
-          <cell r="F46">
+          <cell r="F43">
             <v>40</v>
           </cell>
         </row>
-        <row r="47">
-          <cell r="D47">
+        <row r="44">
+          <cell r="D44">
             <v>100</v>
           </cell>
-          <cell r="E47">
+          <cell r="E44">
             <v>250</v>
           </cell>
-          <cell r="F47">
+          <cell r="F44">
             <v>500</v>
           </cell>
         </row>
-        <row r="48">
-          <cell r="D48">
+        <row r="45">
+          <cell r="D45">
             <v>100</v>
           </cell>
-          <cell r="E48">
+          <cell r="E45">
             <v>250</v>
           </cell>
-          <cell r="F48">
+          <cell r="F45">
             <v>500</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="D49">
+            <v>48000</v>
+          </cell>
+          <cell r="E49">
+            <v>60000</v>
+          </cell>
+          <cell r="F49">
+            <v>80000</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="D50">
+            <v>126000</v>
+          </cell>
+          <cell r="E50">
+            <v>187000</v>
+          </cell>
+          <cell r="F50">
+            <v>249000</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="D51">
+            <v>97000</v>
+          </cell>
+          <cell r="E51">
+            <v>127000</v>
+          </cell>
+          <cell r="F51">
+            <v>158000</v>
           </cell>
         </row>
         <row r="52">
           <cell r="D52">
-            <v>48000</v>
+            <v>53000</v>
           </cell>
           <cell r="E52">
             <v>60000</v>
           </cell>
           <cell r="F52">
-            <v>80000</v>
-          </cell>
-        </row>
-        <row r="53">
-          <cell r="D53">
-            <v>126000</v>
-          </cell>
-          <cell r="E53">
-            <v>187000</v>
-          </cell>
-          <cell r="F53">
-            <v>249000</v>
-          </cell>
-        </row>
-        <row r="54">
-          <cell r="D54">
-            <v>97000</v>
-          </cell>
-          <cell r="E54">
-            <v>127000</v>
-          </cell>
-          <cell r="F54">
-            <v>158000</v>
-          </cell>
-        </row>
-        <row r="55">
-          <cell r="D55">
-            <v>53000</v>
-          </cell>
-          <cell r="E55">
-            <v>60000</v>
-          </cell>
-          <cell r="F55">
             <v>98000</v>
           </cell>
         </row>
@@ -494,6 +494,7 @@
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -801,8 +802,8 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -847,15 +848,15 @@
       </c>
       <c r="B3" s="9">
         <f>'[1]2_assumptions'!D7</f>
-        <v>1464.3</v>
+        <v>1493.3076923076926</v>
       </c>
       <c r="C3" s="10">
         <f>'[1]2_assumptions'!E7</f>
-        <v>1627</v>
+        <v>1659.2307692307695</v>
       </c>
       <c r="D3" s="10">
         <f>'[1]2_assumptions'!F7</f>
-        <v>1789.7</v>
+        <v>1825.1538461538466</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -864,15 +865,15 @@
       </c>
       <c r="B4" s="7">
         <f>'[1]2_assumptions'!D8</f>
-        <v>0.1</v>
+        <v>4.7009735744089003E-2</v>
       </c>
       <c r="C4" s="8">
         <f>'[1]2_assumptions'!E8</f>
-        <v>0.2</v>
+        <v>0.16054705609643019</v>
       </c>
       <c r="D4" s="8">
         <f>'[1]2_assumptions'!F8</f>
-        <v>0.5</v>
+        <v>0.29418173388966151</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -897,15 +898,15 @@
         <v>8</v>
       </c>
       <c r="B6" s="7">
-        <f>'[1]2_assumptions'!D11</f>
+        <f>'[1]2_assumptions'!D10</f>
         <v>0.02</v>
       </c>
-      <c r="C6" s="8">
-        <f>'[1]2_assumptions'!E11</f>
+      <c r="C6" s="7">
+        <f>'[1]2_assumptions'!E10</f>
         <v>0.04</v>
       </c>
-      <c r="D6" s="8">
-        <f>'[1]2_assumptions'!F11</f>
+      <c r="D6" s="7">
+        <f>'[1]2_assumptions'!F10</f>
         <v>0.06</v>
       </c>
     </row>
@@ -914,15 +915,15 @@
         <v>5</v>
       </c>
       <c r="B7" s="11">
-        <f>'[1]2_assumptions'!D12</f>
+        <f>'[1]2_assumptions'!D11</f>
         <v>20</v>
       </c>
-      <c r="C7" s="12">
-        <f>'[1]2_assumptions'!E12</f>
+      <c r="C7" s="11">
+        <f>'[1]2_assumptions'!E11</f>
         <v>35</v>
       </c>
-      <c r="D7" s="12">
-        <f>'[1]2_assumptions'!F12</f>
+      <c r="D7" s="11">
+        <f>'[1]2_assumptions'!F11</f>
         <v>50</v>
       </c>
     </row>
@@ -931,15 +932,15 @@
         <v>6</v>
       </c>
       <c r="B8" s="5">
-        <f>'[1]2_assumptions'!D14</f>
+        <f>'[1]2_assumptions'!D12</f>
         <v>0.05</v>
       </c>
       <c r="C8" s="5">
-        <f>'[1]2_assumptions'!E14</f>
+        <f>'[1]2_assumptions'!E12</f>
         <v>0.15</v>
       </c>
       <c r="D8" s="5">
-        <f>'[1]2_assumptions'!F14</f>
+        <f>'[1]2_assumptions'!F12</f>
         <v>0.25</v>
       </c>
     </row>
@@ -948,15 +949,15 @@
         <v>7</v>
       </c>
       <c r="B9" s="11">
-        <f>'[1]2_assumptions'!D15</f>
+        <f>'[1]2_assumptions'!D13</f>
         <v>50</v>
       </c>
-      <c r="C9" s="12">
-        <f>'[1]2_assumptions'!E15</f>
+      <c r="C9" s="11">
+        <f>'[1]2_assumptions'!E13</f>
         <v>100</v>
       </c>
-      <c r="D9" s="12">
-        <f>'[1]2_assumptions'!F15</f>
+      <c r="D9" s="11">
+        <f>'[1]2_assumptions'!F13</f>
         <v>200</v>
       </c>
     </row>
@@ -976,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136AECFB-FB20-BC48-897E-F1FEDB870F71}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1004,16 +1005,16 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <f>'[1]4_cost_assumptions'!D15</f>
-        <v>37500</v>
+        <f>'[1]4_cost_assumptions'!D16</f>
+        <v>57500</v>
       </c>
       <c r="C2">
-        <f>'[1]4_cost_assumptions'!E15</f>
-        <v>55750</v>
+        <f>'[1]4_cost_assumptions'!E16</f>
+        <v>80750</v>
       </c>
       <c r="D2">
-        <f>'[1]4_cost_assumptions'!F15</f>
-        <v>70250</v>
+        <f>'[1]4_cost_assumptions'!F16</f>
+        <v>105250</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1021,15 +1022,15 @@
         <v>20</v>
       </c>
       <c r="B3">
-        <f>'[1]4_cost_assumptions'!D23</f>
+        <f>'[1]4_cost_assumptions'!D24</f>
         <v>6852</v>
       </c>
       <c r="C3">
-        <f>'[1]4_cost_assumptions'!E23</f>
+        <f>'[1]4_cost_assumptions'!E24</f>
         <v>9312</v>
       </c>
       <c r="D3">
-        <f>'[1]4_cost_assumptions'!F23</f>
+        <f>'[1]4_cost_assumptions'!F24</f>
         <v>17004</v>
       </c>
     </row>
@@ -1038,15 +1039,15 @@
         <v>22</v>
       </c>
       <c r="B4">
-        <f>'[1]4_cost_assumptions'!D28</f>
+        <f>'[1]4_cost_assumptions'!D29</f>
         <v>30</v>
       </c>
       <c r="C4">
-        <f>'[1]4_cost_assumptions'!E28</f>
+        <f>'[1]4_cost_assumptions'!E29</f>
         <v>35</v>
       </c>
       <c r="D4">
-        <f>'[1]4_cost_assumptions'!F28</f>
+        <f>'[1]4_cost_assumptions'!F29</f>
         <v>40</v>
       </c>
     </row>
@@ -1055,15 +1056,15 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <f>'[1]4_cost_assumptions'!D46*365</f>
+        <f>'[1]4_cost_assumptions'!D43*365</f>
         <v>3650</v>
       </c>
       <c r="C5">
-        <f>'[1]4_cost_assumptions'!E46*365</f>
+        <f>'[1]4_cost_assumptions'!E43*365</f>
         <v>9125</v>
       </c>
       <c r="D5">
-        <f>'[1]4_cost_assumptions'!F46*365</f>
+        <f>'[1]4_cost_assumptions'!F43*365</f>
         <v>14600</v>
       </c>
     </row>
@@ -1072,15 +1073,15 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <f>'[1]4_cost_assumptions'!D47*12</f>
+        <f>'[1]4_cost_assumptions'!D44*12</f>
         <v>1200</v>
       </c>
       <c r="C6">
-        <f>'[1]4_cost_assumptions'!E47*12</f>
+        <f>'[1]4_cost_assumptions'!E44*12</f>
         <v>3000</v>
       </c>
       <c r="D6">
-        <f>'[1]4_cost_assumptions'!F47*12</f>
+        <f>'[1]4_cost_assumptions'!F44*12</f>
         <v>6000</v>
       </c>
     </row>
@@ -1089,15 +1090,15 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <f>'[1]4_cost_assumptions'!D48*12</f>
+        <f>'[1]4_cost_assumptions'!D45*12</f>
         <v>1200</v>
       </c>
       <c r="C7">
-        <f>'[1]4_cost_assumptions'!E48*12</f>
+        <f>'[1]4_cost_assumptions'!E45*12</f>
         <v>3000</v>
       </c>
       <c r="D7">
-        <f>'[1]4_cost_assumptions'!F48*12</f>
+        <f>'[1]4_cost_assumptions'!F45*12</f>
         <v>6000</v>
       </c>
     </row>
@@ -1105,16 +1106,16 @@
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
-        <f>'[1]4_cost_assumptions'!D52</f>
+      <c r="B8" s="12">
+        <f>'[1]4_cost_assumptions'!D49</f>
         <v>48000</v>
       </c>
-      <c r="C8">
-        <f>'[1]4_cost_assumptions'!E52</f>
+      <c r="C8" s="12">
+        <f>'[1]4_cost_assumptions'!E49</f>
         <v>60000</v>
       </c>
-      <c r="D8">
-        <f>'[1]4_cost_assumptions'!F52</f>
+      <c r="D8" s="12">
+        <f>'[1]4_cost_assumptions'!F49</f>
         <v>80000</v>
       </c>
     </row>
@@ -1122,16 +1123,16 @@
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <f>'[1]4_cost_assumptions'!D53</f>
+      <c r="B9" s="12">
+        <f>'[1]4_cost_assumptions'!D50</f>
         <v>126000</v>
       </c>
-      <c r="C9">
-        <f>'[1]4_cost_assumptions'!E53</f>
+      <c r="C9" s="12">
+        <f>'[1]4_cost_assumptions'!E50</f>
         <v>187000</v>
       </c>
-      <c r="D9">
-        <f>'[1]4_cost_assumptions'!F53</f>
+      <c r="D9" s="12">
+        <f>'[1]4_cost_assumptions'!F50</f>
         <v>249000</v>
       </c>
     </row>
@@ -1139,16 +1140,16 @@
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
-        <f>'[1]4_cost_assumptions'!D54</f>
+      <c r="B10" s="12">
+        <f>'[1]4_cost_assumptions'!D51</f>
         <v>97000</v>
       </c>
-      <c r="C10">
-        <f>'[1]4_cost_assumptions'!E54</f>
+      <c r="C10" s="12">
+        <f>'[1]4_cost_assumptions'!E51</f>
         <v>127000</v>
       </c>
-      <c r="D10">
-        <f>'[1]4_cost_assumptions'!F54</f>
+      <c r="D10" s="12">
+        <f>'[1]4_cost_assumptions'!F51</f>
         <v>158000</v>
       </c>
     </row>
@@ -1156,16 +1157,16 @@
       <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
-        <f>'[1]4_cost_assumptions'!D55</f>
+      <c r="B11" s="12">
+        <f>'[1]4_cost_assumptions'!D52</f>
         <v>53000</v>
       </c>
-      <c r="C11">
-        <f>'[1]4_cost_assumptions'!E55</f>
+      <c r="C11" s="12">
+        <f>'[1]4_cost_assumptions'!E52</f>
         <v>60000</v>
       </c>
-      <c r="D11">
-        <f>'[1]4_cost_assumptions'!F55</f>
+      <c r="D11" s="12">
+        <f>'[1]4_cost_assumptions'!F52</f>
         <v>98000</v>
       </c>
     </row>
@@ -1179,10 +1180,13 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1206,7 +1210,7 @@
         <v>19</v>
       </c>
       <c r="B3">
-        <f>'[1]4_cost_assumptions'!E36</f>
+        <f>'[1]4_cost_assumptions'!E34</f>
         <v>25</v>
       </c>
     </row>
@@ -1214,8 +1218,8 @@
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4">
-        <f>'[1]4_cost_assumptions'!E41</f>
+      <c r="B4" s="13">
+        <f>'[1]4_cost_assumptions'!E38</f>
         <v>0.3</v>
       </c>
     </row>
@@ -1224,7 +1228,7 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <f>'[1]4_cost_assumptions'!E42</f>
+        <f>'[1]4_cost_assumptions'!E39</f>
         <v>2.5999999999999999E-2</v>
       </c>
     </row>

</xml_diff>